<commit_message>
Inclusion of Natural Hazard data for the Inform Risk Index
</commit_message>
<xml_diff>
--- a/Risk_sheets/Indicator aggregation.xlsx
+++ b/Risk_sheets/Indicator aggregation.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ljmac/Google Drive/PhD/R code/Compound Risk/Compound Risk/covid/compoundriskdata/Risk_sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0A48D87-AD10-6146-AA67-F0087C29F4AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B53EA7F2-D5E8-144D-B92F-85FF3486AB0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{B42EF1BE-965E-B741-ADF0-C68AD4A5C459}"/>
+    <workbookView xWindow="40" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{B42EF1BE-965E-B741-ADF0-C68AD4A5C459}"/>
   </bookViews>
   <sheets>
-    <sheet name="Risk Components" sheetId="1" r:id="rId1"/>
-    <sheet name="Total Risk" sheetId="2" r:id="rId2"/>
+    <sheet name="Emerging Risk" sheetId="1" r:id="rId1"/>
+    <sheet name="Existing Risk" sheetId="3" r:id="rId2"/>
+    <sheet name="Total Risk" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="131">
   <si>
     <r>
       <t xml:space="preserve">Growth in conflict fatalities - </t>
@@ -296,12 +297,6 @@
   </si>
   <si>
     <t>F_Fewsnet_Score_norm</t>
-  </si>
-  <si>
-    <t>C_ACLED_event_same_month_difference_perc_norm</t>
-  </si>
-  <si>
-    <t>C_ACLED_fatal_same_month_difference_perc_norm</t>
   </si>
   <si>
     <t>Fr_FSI_2019minus2020_norm</t>
@@ -744,10 +739,6 @@
 0 &lt; 0</t>
   </si>
   <si>
-    <t>10 &lt; 90 pct 
-0 &gt;  pct</t>
-  </si>
-  <si>
     <t>10 &lt; 20 pct
 0 &gt; 95 pct</t>
   </si>
@@ -1121,13 +1112,147 @@
   </si>
   <si>
     <t>`</t>
+  </si>
+  <si>
+    <t>Fr_ACLED_event_same_month_difference_perc_norm</t>
+  </si>
+  <si>
+    <t>Fr_ACLED_fatal_same_month_difference_perc_norm</t>
+  </si>
+  <si>
+    <t>Fr_INFORM_Fragility_Score</t>
+  </si>
+  <si>
+    <t>INFORM institutional score</t>
+  </si>
+  <si>
+    <t>10 &lt; 95 pct 
+0 &gt; 5 pct</t>
+  </si>
+  <si>
+    <t>10 &lt; 90 pct 
+0 &gt; 10 pct</t>
+  </si>
+  <si>
+    <t>H_HIS_Score_norm</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>F_Proteus_Score_norm</t>
+  </si>
+  <si>
+    <t>M_Economic_and_Financial_score_norm</t>
+  </si>
+  <si>
+    <t>D_WB_Overall_debt_distress_norm</t>
+  </si>
+  <si>
+    <t>S_OCHA_Covid.vulnerability.index_norm</t>
+  </si>
+  <si>
+    <t>Fr_WB_structural_norm</t>
+  </si>
+  <si>
+    <t>SOCIOECONOMIC VULNERABILITY RISK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 &gt;= 20 
+0 &lt;=  70 </t>
+  </si>
+  <si>
+    <t>WFP Proteus composite index, measuring multidimensional aspects of food security</t>
+  </si>
+  <si>
+    <t>WB's structural conflict model comprised of a range of fragility-related source indicators</t>
+  </si>
+  <si>
+    <t>Numeric average of composite scores for Economic Dependence and Financial Dependence</t>
+  </si>
+  <si>
+    <t>WB measure of overall debt distress</t>
+  </si>
+  <si>
+    <t>Global Health Score Index, a composite index made up of a variety of health-related indicators</t>
+  </si>
+  <si>
+    <t>Composite Index comprised of a range of socio-economic variables compiled by UNOCHA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 &gt;= 95 pct 
+0 &lt;=  5 pct </t>
+  </si>
+  <si>
+    <t>10 = In distress OR high
+7 = Moderate
+3 = Low</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 &gt;= 90 pct 
+0 &lt;= 10 pct </t>
+  </si>
+  <si>
+    <t>AGGREGATION</t>
+  </si>
+  <si>
+    <t>F = F_Proteus_Score_norm</t>
+  </si>
+  <si>
+    <t>D = D_WB_Overall_debt_distress_norm</t>
+  </si>
+  <si>
+    <t>i.           Poverty    
+ii.           Multidimensional Poverty Index  
+iii.           Human Development Index     
+ix.           Population living in slums (% of urban population) 
+iv.           Internal connectedness (Road density)    
+v.           Access to cities  
+vi.           Displaced population 
+vii.           IDP, refugees and returnees [percentage of population] 
+viii.           Household size   
+ix.           Population living in slums (% of urban population) 
+x.           Population living in urban areas
+xii.           Social protection adequacy (ASPIRE) – added  
+xiii.           Social Protection coverage (ASPIRE) – added</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Social Protection = 
+Poverty = 
+Density Index = 
+Movement = 
+--------------------------------------
+Risk Factors = 
+Transmission = 
+----------------------------------------
+Socio-economic Vulnerability = </t>
+  </si>
+  <si>
+    <t>SOURCE INDICATORS</t>
+  </si>
+  <si>
+    <t>i.	Fuel imports (% of merchandise imports) 2018
+ii.	Food imports (% of merchandise imports) 2018	
+iii.	Travel and Tourism total contribution to GDP, Percentage share of total GDP, 2019
+iv.	Net ODA received (% of central government expense) 2017
+v.	Personal remittances, received (% of GDP) 2017	
+vi.	Total reserves in months of imports 2016	
+vii.	Gross savings (% of GDP) 2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">min-max normalization for each variable (with high/low thresholds assigned)
+Economic dependence = 
+Financial capacity = 
+----------------------------------------
+Macro = max(ED, FC)
+</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1200,8 +1325,37 @@
       <name val="Garamond"/>
       <family val="1"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Garamond"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color rgb="FF000000"/>
+      <name val="Garamond"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="16">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1292,8 +1446,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -1421,11 +1587,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1533,6 +1709,57 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1543,15 +1770,9 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1563,53 +1784,48 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="6"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="6"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1623,6 +1839,650 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2136448</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>261122</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2847648</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>488298</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6BE9FCC-379D-C848-8610-090D330B7551}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="15691027" y="5020655"/>
+          <a:ext cx="711200" cy="227176"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1994019</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>652803</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2768719</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>879979</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20843FAA-B700-E24A-BD85-A88D187D2A96}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="15548598" y="5412336"/>
+          <a:ext cx="774700" cy="227176"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2077103</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>1044486</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>477852</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>1271661</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7D7F387E-F96E-3443-8DC8-48AEBCA64519}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="15631682" y="5804019"/>
+          <a:ext cx="1498600" cy="227175"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2053365</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>1483645</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2599465</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>1710821</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DD4954E5-9D71-D947-8C22-EF6B4423CE54}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="15607944" y="6243178"/>
+          <a:ext cx="546100" cy="227176"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2100841</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>1863457</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2786641</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>2103333</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D6E55DF2-3DA7-B848-8718-242DBA10213D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="15655420" y="6622990"/>
+          <a:ext cx="685800" cy="239876"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2100840</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>2267010</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2735840</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>2506886</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CFE0D66F-DBA9-4249-A6F4-2CDE36487BE0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="15655419" y="7026543"/>
+          <a:ext cx="635000" cy="239876"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2480654</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>2682430</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>17803</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>2922305</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE947BBC-0B9D-BD40-9960-E13C70E08CB1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="16035233" y="7441963"/>
+          <a:ext cx="635000" cy="239875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1388691</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>818972</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1922091</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>1046148</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Picture 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1A8A7F1F-9AC1-DB41-84EB-AB030C9C5D2A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="15192523" y="2836729"/>
+          <a:ext cx="533400" cy="227176"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1210654</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>1210655</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1858354</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>1437831</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Picture 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E662A1F4-E1AF-1741-A5D8-F8C830E7EAF7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="15014486" y="3228412"/>
+          <a:ext cx="647700" cy="227176"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1923,12 +2783,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A43FA0A0-CA91-8045-A959-B8DB842256EB}">
   <sheetPr>
-    <tabColor theme="7" tint="0.79998168889431442"/>
+    <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:CR28"/>
+  <dimension ref="A1:CR29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="89" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView zoomScale="89" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1951,7 +2811,7 @@
         <v>20</v>
       </c>
       <c r="C1" s="23" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D1" s="35" t="s">
         <v>9</v>
@@ -1964,14 +2824,14 @@
       </c>
     </row>
     <row r="2" spans="1:96" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="41" t="s">
-        <v>47</v>
-      </c>
-      <c r="B2" s="42"/>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="43"/>
+      <c r="A2" s="58" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="59"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="60"/>
       <c r="G2" s="15"/>
       <c r="H2" s="15"/>
       <c r="I2" s="15"/>
@@ -2068,19 +2928,19 @@
         <v>24</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>78</v>
-      </c>
-      <c r="D3" s="51" t="s">
-        <v>63</v>
-      </c>
-      <c r="E3" s="51" t="s">
-        <v>95</v>
-      </c>
-      <c r="F3" s="48" t="s">
-        <v>64</v>
+        <v>76</v>
+      </c>
+      <c r="D3" s="54" t="s">
+        <v>61</v>
+      </c>
+      <c r="E3" s="54" t="s">
+        <v>92</v>
+      </c>
+      <c r="F3" s="63" t="s">
+        <v>62</v>
       </c>
       <c r="G3" s="15"/>
       <c r="H3" s="15"/>
@@ -2178,14 +3038,14 @@
         <v>26</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
-      <c r="F4" s="48"/>
+        <v>75</v>
+      </c>
+      <c r="D4" s="54"/>
+      <c r="E4" s="54"/>
+      <c r="F4" s="63"/>
       <c r="G4" s="15"/>
       <c r="H4" s="15"/>
       <c r="I4" s="15"/>
@@ -2282,14 +3142,14 @@
         <v>25</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>79</v>
-      </c>
-      <c r="D5" s="51"/>
-      <c r="E5" s="51"/>
-      <c r="F5" s="48"/>
+        <v>77</v>
+      </c>
+      <c r="D5" s="54"/>
+      <c r="E5" s="54"/>
+      <c r="F5" s="63"/>
       <c r="G5" s="15"/>
       <c r="H5" s="15"/>
       <c r="I5" s="15"/>
@@ -2381,14 +3241,14 @@
       <c r="CQ5" s="15"/>
     </row>
     <row r="6" spans="1:96" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="41" t="s">
-        <v>92</v>
-      </c>
-      <c r="B6" s="42"/>
-      <c r="C6" s="42"/>
-      <c r="D6" s="42"/>
-      <c r="E6" s="42"/>
-      <c r="F6" s="43"/>
+      <c r="A6" s="58" t="s">
+        <v>89</v>
+      </c>
+      <c r="B6" s="59"/>
+      <c r="C6" s="59"/>
+      <c r="D6" s="59"/>
+      <c r="E6" s="59"/>
+      <c r="F6" s="60"/>
       <c r="G6" s="15"/>
       <c r="H6" s="15"/>
       <c r="I6" s="15"/>
@@ -2481,22 +3341,22 @@
     </row>
     <row r="7" spans="1:96" s="2" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
-        <v>27</v>
+        <v>99</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="D7" s="53" t="s">
+        <v>78</v>
+      </c>
+      <c r="D7" s="44" t="s">
+        <v>90</v>
+      </c>
+      <c r="E7" s="44" t="s">
         <v>93</v>
       </c>
-      <c r="E7" s="53" t="s">
-        <v>96</v>
-      </c>
-      <c r="F7" s="57" t="s">
-        <v>94</v>
+      <c r="F7" s="41" t="s">
+        <v>91</v>
       </c>
       <c r="G7" s="15"/>
       <c r="H7" s="15"/>
@@ -2590,17 +3450,17 @@
     </row>
     <row r="8" spans="1:96" s="2" customFormat="1" ht="49" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
-        <v>28</v>
+        <v>100</v>
       </c>
       <c r="B8" s="11" t="s">
         <v>0</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>81</v>
-      </c>
-      <c r="D8" s="55"/>
-      <c r="E8" s="55"/>
-      <c r="F8" s="58"/>
+        <v>79</v>
+      </c>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="42"/>
       <c r="G8" s="15"/>
       <c r="H8" s="15"/>
       <c r="I8" s="15"/>
@@ -2693,17 +3553,17 @@
     </row>
     <row r="9" spans="1:96" s="3" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C9" s="40" t="s">
-        <v>82</v>
-      </c>
-      <c r="D9" s="55"/>
-      <c r="E9" s="55"/>
-      <c r="F9" s="58"/>
+        <v>104</v>
+      </c>
+      <c r="D9" s="45"/>
+      <c r="E9" s="45"/>
+      <c r="F9" s="42"/>
       <c r="G9" s="15"/>
       <c r="H9" s="15"/>
       <c r="I9" s="15"/>
@@ -2796,17 +3656,17 @@
     </row>
     <row r="10" spans="1:96" s="3" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="40" t="s">
-        <v>90</v>
-      </c>
-      <c r="D10" s="55"/>
-      <c r="E10" s="55"/>
-      <c r="F10" s="58"/>
+        <v>87</v>
+      </c>
+      <c r="D10" s="45"/>
+      <c r="E10" s="45"/>
+      <c r="F10" s="42"/>
       <c r="G10" s="15"/>
       <c r="H10" s="15"/>
       <c r="I10" s="15"/>
@@ -2899,17 +3759,17 @@
     </row>
     <row r="11" spans="1:96" s="3" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="17" t="s">
-        <v>30</v>
+        <v>101</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>1</v>
+        <v>102</v>
       </c>
       <c r="C11" s="40" t="s">
-        <v>82</v>
-      </c>
-      <c r="D11" s="54"/>
-      <c r="E11" s="54"/>
-      <c r="F11" s="59"/>
+        <v>103</v>
+      </c>
+      <c r="D11" s="45"/>
+      <c r="E11" s="45"/>
+      <c r="F11" s="42"/>
       <c r="G11" s="15"/>
       <c r="H11" s="15"/>
       <c r="I11" s="15"/>
@@ -3000,15 +3860,19 @@
       <c r="CP11" s="15"/>
       <c r="CQ11" s="15"/>
     </row>
-    <row r="12" spans="1:96" s="3" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="47" t="s">
-        <v>62</v>
-      </c>
-      <c r="B12" s="56"/>
-      <c r="C12" s="56"/>
-      <c r="D12" s="56"/>
-      <c r="E12" s="56"/>
-      <c r="F12" s="56"/>
+    <row r="12" spans="1:96" s="3" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A12" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="40" t="s">
+        <v>103</v>
+      </c>
+      <c r="D12" s="46"/>
+      <c r="E12" s="46"/>
+      <c r="F12" s="43"/>
       <c r="G12" s="15"/>
       <c r="H12" s="15"/>
       <c r="I12" s="15"/>
@@ -3099,25 +3963,15 @@
       <c r="CP12" s="15"/>
       <c r="CQ12" s="15"/>
     </row>
-    <row r="13" spans="1:96" s="3" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="C13" s="22" t="s">
-        <v>83</v>
-      </c>
-      <c r="D13" s="51" t="s">
-        <v>13</v>
-      </c>
-      <c r="E13" s="51" t="s">
-        <v>14</v>
-      </c>
-      <c r="F13" s="49" t="s">
-        <v>15</v>
-      </c>
+    <row r="13" spans="1:96" s="3" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="61" t="s">
+        <v>60</v>
+      </c>
+      <c r="B13" s="62"/>
+      <c r="C13" s="62"/>
+      <c r="D13" s="62"/>
+      <c r="E13" s="62"/>
+      <c r="F13" s="62"/>
       <c r="G13" s="15"/>
       <c r="H13" s="15"/>
       <c r="I13" s="15"/>
@@ -3208,19 +4062,25 @@
       <c r="CP13" s="15"/>
       <c r="CQ13" s="15"/>
     </row>
-    <row r="14" spans="1:96" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:96" s="3" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>83</v>
-      </c>
-      <c r="D14" s="51"/>
-      <c r="E14" s="51"/>
-      <c r="F14" s="49"/>
+        <v>80</v>
+      </c>
+      <c r="D14" s="54" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="54" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" s="64" t="s">
+        <v>15</v>
+      </c>
       <c r="G14" s="15"/>
       <c r="H14" s="15"/>
       <c r="I14" s="15"/>
@@ -3311,15 +4171,19 @@
       <c r="CP14" s="15"/>
       <c r="CQ14" s="15"/>
     </row>
-    <row r="15" spans="1:96" s="4" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="41" t="s">
-        <v>48</v>
-      </c>
-      <c r="B15" s="42"/>
-      <c r="C15" s="42"/>
-      <c r="D15" s="42"/>
-      <c r="E15" s="42"/>
-      <c r="F15" s="43"/>
+    <row r="15" spans="1:96" s="3" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A15" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="D15" s="54"/>
+      <c r="E15" s="54"/>
+      <c r="F15" s="64"/>
       <c r="G15" s="15"/>
       <c r="H15" s="15"/>
       <c r="I15" s="15"/>
@@ -3409,27 +4273,16 @@
       <c r="CO15" s="15"/>
       <c r="CP15" s="15"/>
       <c r="CQ15" s="15"/>
-      <c r="CR15" s="15"/>
     </row>
-    <row r="16" spans="1:96" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A16" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="B16" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="C16" s="31" t="s">
-        <v>84</v>
-      </c>
-      <c r="D16" s="32" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" s="32" t="s">
-        <v>97</v>
-      </c>
-      <c r="F16" s="33" t="s">
-        <v>16</v>
-      </c>
+    <row r="16" spans="1:96" s="4" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="58" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" s="59"/>
+      <c r="C16" s="59"/>
+      <c r="D16" s="59"/>
+      <c r="E16" s="59"/>
+      <c r="F16" s="60"/>
       <c r="G16" s="15"/>
       <c r="H16" s="15"/>
       <c r="I16" s="15"/>
@@ -3521,15 +4374,25 @@
       <c r="CQ16" s="15"/>
       <c r="CR16" s="15"/>
     </row>
-    <row r="17" spans="1:96" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="47" t="s">
-        <v>61</v>
-      </c>
-      <c r="B17" s="56"/>
-      <c r="C17" s="56"/>
-      <c r="D17" s="56"/>
-      <c r="E17" s="56"/>
-      <c r="F17" s="56"/>
+    <row r="17" spans="1:96" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A17" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="C17" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="D17" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="32" t="s">
+        <v>94</v>
+      </c>
+      <c r="F17" s="33" t="s">
+        <v>16</v>
+      </c>
       <c r="G17" s="15"/>
       <c r="H17" s="15"/>
       <c r="I17" s="15"/>
@@ -3621,25 +4484,15 @@
       <c r="CQ17" s="15"/>
       <c r="CR17" s="15"/>
     </row>
-    <row r="18" spans="1:96" s="4" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="B18" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="C18" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="D18" s="52" t="s">
-        <v>17</v>
-      </c>
-      <c r="E18" s="52" t="s">
-        <v>18</v>
-      </c>
-      <c r="F18" s="50" t="s">
-        <v>19</v>
-      </c>
+    <row r="18" spans="1:96" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="61" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" s="62"/>
+      <c r="C18" s="62"/>
+      <c r="D18" s="62"/>
+      <c r="E18" s="62"/>
+      <c r="F18" s="62"/>
       <c r="G18" s="15"/>
       <c r="H18" s="15"/>
       <c r="I18" s="15"/>
@@ -3731,19 +4584,25 @@
       <c r="CQ18" s="15"/>
       <c r="CR18" s="15"/>
     </row>
-    <row r="19" spans="1:96" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:96" s="4" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="B19" s="12" t="s">
-        <v>2</v>
+        <v>38</v>
+      </c>
+      <c r="B19" s="28" t="s">
+        <v>56</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="D19" s="52"/>
-      <c r="E19" s="52"/>
-      <c r="F19" s="50"/>
+        <v>82</v>
+      </c>
+      <c r="D19" s="53" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19" s="53" t="s">
+        <v>18</v>
+      </c>
+      <c r="F19" s="65" t="s">
+        <v>19</v>
+      </c>
       <c r="G19" s="15"/>
       <c r="H19" s="15"/>
       <c r="I19" s="15"/>
@@ -3837,21 +4696,19 @@
     </row>
     <row r="20" spans="1:96" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" s="18" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="D20" s="52"/>
-      <c r="E20" s="52"/>
-      <c r="F20" s="50"/>
+        <v>83</v>
+      </c>
+      <c r="D20" s="53"/>
+      <c r="E20" s="53"/>
+      <c r="F20" s="65"/>
       <c r="G20" s="15"/>
-      <c r="H20" s="15" t="s">
-        <v>101</v>
-      </c>
+      <c r="H20" s="15"/>
       <c r="I20" s="15"/>
       <c r="J20" s="15"/>
       <c r="K20" s="15"/>
@@ -3943,19 +4800,21 @@
     </row>
     <row r="21" spans="1:96" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" s="18" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="D21" s="52"/>
-      <c r="E21" s="52"/>
-      <c r="F21" s="50"/>
+        <v>83</v>
+      </c>
+      <c r="D21" s="53"/>
+      <c r="E21" s="53"/>
+      <c r="F21" s="65"/>
       <c r="G21" s="15"/>
-      <c r="H21" s="15"/>
+      <c r="H21" s="15" t="s">
+        <v>98</v>
+      </c>
       <c r="I21" s="15"/>
       <c r="J21" s="15"/>
       <c r="K21" s="15"/>
@@ -4047,17 +4906,17 @@
     </row>
     <row r="22" spans="1:96" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" s="18" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="D22" s="52"/>
-      <c r="E22" s="52"/>
-      <c r="F22" s="50"/>
+        <v>84</v>
+      </c>
+      <c r="D22" s="53"/>
+      <c r="E22" s="53"/>
+      <c r="F22" s="65"/>
       <c r="G22" s="15"/>
       <c r="H22" s="15"/>
       <c r="I22" s="15"/>
@@ -4151,17 +5010,17 @@
     </row>
     <row r="23" spans="1:96" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" s="18" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>59</v>
+        <v>5</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="D23" s="52"/>
-      <c r="E23" s="52"/>
-      <c r="F23" s="50"/>
+        <v>85</v>
+      </c>
+      <c r="D23" s="53"/>
+      <c r="E23" s="53"/>
+      <c r="F23" s="65"/>
       <c r="G23" s="15"/>
       <c r="H23" s="15"/>
       <c r="I23" s="15"/>
@@ -4253,15 +5112,19 @@
       <c r="CQ23" s="15"/>
       <c r="CR23" s="15"/>
     </row>
-    <row r="24" spans="1:96" s="5" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="44" t="s">
-        <v>49</v>
-      </c>
-      <c r="B24" s="45"/>
-      <c r="C24" s="45"/>
-      <c r="D24" s="45"/>
-      <c r="E24" s="45"/>
-      <c r="F24" s="46"/>
+    <row r="24" spans="1:96" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A24" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="D24" s="53"/>
+      <c r="E24" s="53"/>
+      <c r="F24" s="65"/>
       <c r="G24" s="15"/>
       <c r="H24" s="15"/>
       <c r="I24" s="15"/>
@@ -4353,25 +5216,15 @@
       <c r="CQ24" s="15"/>
       <c r="CR24" s="15"/>
     </row>
-    <row r="25" spans="1:96" s="5" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="B25" s="29" t="s">
-        <v>60</v>
-      </c>
-      <c r="C25" s="25" t="s">
-        <v>89</v>
-      </c>
-      <c r="D25" s="60" t="s">
-        <v>98</v>
-      </c>
-      <c r="E25" s="60" t="s">
-        <v>99</v>
-      </c>
-      <c r="F25" s="63" t="s">
-        <v>100</v>
-      </c>
+    <row r="25" spans="1:96" s="5" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="55" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" s="56"/>
+      <c r="C25" s="56"/>
+      <c r="D25" s="56"/>
+      <c r="E25" s="56"/>
+      <c r="F25" s="57"/>
       <c r="G25" s="15"/>
       <c r="H25" s="15"/>
       <c r="I25" s="15"/>
@@ -4463,19 +5316,25 @@
       <c r="CQ25" s="15"/>
       <c r="CR25" s="15"/>
     </row>
-    <row r="26" spans="1:96" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:96" s="5" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="B26" s="14" t="s">
-        <v>6</v>
+        <v>39</v>
+      </c>
+      <c r="B26" s="29" t="s">
+        <v>58</v>
       </c>
       <c r="C26" s="25" t="s">
-        <v>91</v>
-      </c>
-      <c r="D26" s="61"/>
-      <c r="E26" s="61"/>
-      <c r="F26" s="64"/>
+        <v>86</v>
+      </c>
+      <c r="D26" s="47" t="s">
+        <v>95</v>
+      </c>
+      <c r="E26" s="47" t="s">
+        <v>96</v>
+      </c>
+      <c r="F26" s="50" t="s">
+        <v>97</v>
+      </c>
       <c r="G26" s="15"/>
       <c r="H26" s="15"/>
       <c r="I26" s="15"/>
@@ -4569,17 +5428,17 @@
     </row>
     <row r="27" spans="1:96" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" s="19" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>43</v>
+        <v>6</v>
       </c>
       <c r="C27" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="D27" s="62"/>
-      <c r="E27" s="62"/>
-      <c r="F27" s="65"/>
+        <v>88</v>
+      </c>
+      <c r="D27" s="48"/>
+      <c r="E27" s="48"/>
+      <c r="F27" s="51"/>
       <c r="G27" s="15"/>
       <c r="H27" s="15"/>
       <c r="I27" s="15"/>
@@ -4671,43 +5530,147 @@
       <c r="CQ27" s="15"/>
       <c r="CR27" s="15"/>
     </row>
-    <row r="28" spans="1:96" ht="51" x14ac:dyDescent="0.2">
-      <c r="C28" s="20" t="s">
+    <row r="28" spans="1:96" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A28" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C28" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="D28" s="49"/>
+      <c r="E28" s="49"/>
+      <c r="F28" s="52"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="15"/>
+      <c r="I28" s="15"/>
+      <c r="J28" s="15"/>
+      <c r="K28" s="15"/>
+      <c r="L28" s="15"/>
+      <c r="M28" s="15"/>
+      <c r="N28" s="15"/>
+      <c r="O28" s="15"/>
+      <c r="P28" s="15"/>
+      <c r="Q28" s="15"/>
+      <c r="R28" s="15"/>
+      <c r="S28" s="15"/>
+      <c r="T28" s="15"/>
+      <c r="U28" s="15"/>
+      <c r="V28" s="15"/>
+      <c r="W28" s="15"/>
+      <c r="X28" s="15"/>
+      <c r="Y28" s="15"/>
+      <c r="Z28" s="15"/>
+      <c r="AA28" s="15"/>
+      <c r="AB28" s="15"/>
+      <c r="AC28" s="15"/>
+      <c r="AD28" s="15"/>
+      <c r="AE28" s="15"/>
+      <c r="AF28" s="15"/>
+      <c r="AG28" s="15"/>
+      <c r="AH28" s="15"/>
+      <c r="AI28" s="15"/>
+      <c r="AJ28" s="15"/>
+      <c r="AK28" s="15"/>
+      <c r="AL28" s="15"/>
+      <c r="AM28" s="15"/>
+      <c r="AN28" s="15"/>
+      <c r="AO28" s="15"/>
+      <c r="AP28" s="15"/>
+      <c r="AQ28" s="15"/>
+      <c r="AR28" s="15"/>
+      <c r="AS28" s="15"/>
+      <c r="AT28" s="15"/>
+      <c r="AU28" s="15"/>
+      <c r="AV28" s="15"/>
+      <c r="AW28" s="15"/>
+      <c r="AX28" s="15"/>
+      <c r="AY28" s="15"/>
+      <c r="AZ28" s="15"/>
+      <c r="BA28" s="15"/>
+      <c r="BB28" s="15"/>
+      <c r="BC28" s="15"/>
+      <c r="BD28" s="15"/>
+      <c r="BE28" s="15"/>
+      <c r="BF28" s="15"/>
+      <c r="BG28" s="15"/>
+      <c r="BH28" s="15"/>
+      <c r="BI28" s="15"/>
+      <c r="BJ28" s="15"/>
+      <c r="BK28" s="15"/>
+      <c r="BL28" s="15"/>
+      <c r="BM28" s="15"/>
+      <c r="BN28" s="15"/>
+      <c r="BO28" s="15"/>
+      <c r="BP28" s="15"/>
+      <c r="BQ28" s="15"/>
+      <c r="BR28" s="15"/>
+      <c r="BS28" s="15"/>
+      <c r="BT28" s="15"/>
+      <c r="BU28" s="15"/>
+      <c r="BV28" s="15"/>
+      <c r="BW28" s="15"/>
+      <c r="BX28" s="15"/>
+      <c r="BY28" s="15"/>
+      <c r="BZ28" s="15"/>
+      <c r="CA28" s="15"/>
+      <c r="CB28" s="15"/>
+      <c r="CC28" s="15"/>
+      <c r="CD28" s="15"/>
+      <c r="CE28" s="15"/>
+      <c r="CF28" s="15"/>
+      <c r="CG28" s="15"/>
+      <c r="CH28" s="15"/>
+      <c r="CI28" s="15"/>
+      <c r="CJ28" s="15"/>
+      <c r="CK28" s="15"/>
+      <c r="CL28" s="15"/>
+      <c r="CM28" s="15"/>
+      <c r="CN28" s="15"/>
+      <c r="CO28" s="15"/>
+      <c r="CP28" s="15"/>
+      <c r="CQ28" s="15"/>
+      <c r="CR28" s="15"/>
+    </row>
+    <row r="29" spans="1:96" ht="51" x14ac:dyDescent="0.2">
+      <c r="C29" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="D28" s="21" t="s">
+      <c r="D29" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="E28" s="21" t="s">
+      <c r="E29" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="F28" s="21" t="s">
+      <c r="F29" s="21" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="F7:F11"/>
-    <mergeCell ref="E7:E11"/>
-    <mergeCell ref="D25:D27"/>
-    <mergeCell ref="E25:E27"/>
-    <mergeCell ref="F25:F27"/>
-    <mergeCell ref="D18:D23"/>
-    <mergeCell ref="E3:E5"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="E18:E23"/>
-    <mergeCell ref="D7:D11"/>
-    <mergeCell ref="A24:F24"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A6:F6"/>
-    <mergeCell ref="A15:F15"/>
-    <mergeCell ref="A17:F17"/>
-    <mergeCell ref="A12:F12"/>
+    <mergeCell ref="A16:F16"/>
+    <mergeCell ref="A18:F18"/>
+    <mergeCell ref="A13:F13"/>
     <mergeCell ref="F3:F5"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="F18:F23"/>
+    <mergeCell ref="F14:F15"/>
     <mergeCell ref="D3:D5"/>
-    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E3:E5"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="E19:E24"/>
+    <mergeCell ref="D7:D12"/>
+    <mergeCell ref="A25:F25"/>
+    <mergeCell ref="F19:F24"/>
+    <mergeCell ref="F7:F12"/>
+    <mergeCell ref="E7:E12"/>
+    <mergeCell ref="D26:D28"/>
+    <mergeCell ref="E26:E28"/>
+    <mergeCell ref="F26:F28"/>
+    <mergeCell ref="D19:D24"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -4715,25 +5678,256 @@
     <hyperlink ref="B4" r:id="rId2" display="https://fews.net/" xr:uid="{84772C4A-4AD9-7840-815D-17F2F6B2D9A0}"/>
     <hyperlink ref="B7" r:id="rId3" location="/dashboard" display="https://acleddata.com/dashboard/ - /dashboard" xr:uid="{F76E7675-2B2E-2D45-8C2B-2CB43E3D6E32}"/>
     <hyperlink ref="B9" r:id="rId4" display="https://fragilestatesindex.org/data/" xr:uid="{A9B1CC3D-C0A1-C04F-BBD3-3E6A6BCE7B20}"/>
-    <hyperlink ref="B11" r:id="rId5" display="https://oefdatascience.github.io/REIGN.github.io/" xr:uid="{2AEFFF55-2CCA-7F42-82FE-4DED88CAF0DE}"/>
-    <hyperlink ref="B13" r:id="rId6" display="https://www.worldbank.org/en/publication/global-economic-prospects" xr:uid="{6B81CDE3-78BD-FB41-88E5-D7CCF55FBF33}"/>
-    <hyperlink ref="B14" r:id="rId7" display="https://www.imf.org/external/pubs/ft/weo/2020/01/weodata/download.aspx" xr:uid="{283F4A21-AE52-424B-A454-2015ED782078}"/>
-    <hyperlink ref="B16" r:id="rId8" display="https://www.imf.org/external/pubs/ft/weo/2020/01/weodata/download.aspx" xr:uid="{A46374A5-6C1D-3A40-9101-CF1B60D6931C}"/>
-    <hyperlink ref="B23" r:id="rId9" display="https://www.bsg.ox.ac.uk/research/publications/lockdown-rollback-checklist" xr:uid="{859F7DF3-36B6-344E-923B-6E65426E76CD}"/>
+    <hyperlink ref="B12" r:id="rId5" display="https://oefdatascience.github.io/REIGN.github.io/" xr:uid="{2AEFFF55-2CCA-7F42-82FE-4DED88CAF0DE}"/>
+    <hyperlink ref="B14" r:id="rId6" display="https://www.worldbank.org/en/publication/global-economic-prospects" xr:uid="{6B81CDE3-78BD-FB41-88E5-D7CCF55FBF33}"/>
+    <hyperlink ref="B15" r:id="rId7" display="https://www.imf.org/external/pubs/ft/weo/2020/01/weodata/download.aspx" xr:uid="{283F4A21-AE52-424B-A454-2015ED782078}"/>
+    <hyperlink ref="B17" r:id="rId8" display="https://www.imf.org/external/pubs/ft/weo/2020/01/weodata/download.aspx" xr:uid="{A46374A5-6C1D-3A40-9101-CF1B60D6931C}"/>
+    <hyperlink ref="B24" r:id="rId9" display="https://www.bsg.ox.ac.uk/research/publications/lockdown-rollback-checklist" xr:uid="{859F7DF3-36B6-344E-923B-6E65426E76CD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF80EE09-2355-2249-B578-564806843C25}">
+  <sheetPr>
+    <tabColor theme="2" tint="-9.9978637043366805E-2"/>
+  </sheetPr>
+  <dimension ref="A1:G15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="107" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="41.5" customWidth="1"/>
+    <col min="2" max="2" width="53" customWidth="1"/>
+    <col min="3" max="3" width="24.5" customWidth="1"/>
+    <col min="4" max="4" width="62.33203125" customWidth="1"/>
+    <col min="5" max="5" width="40.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="35" t="s">
+        <v>128</v>
+      </c>
+      <c r="E1" s="35" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="58" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="59"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+    </row>
+    <row r="3" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="B3" s="72" t="s">
+        <v>114</v>
+      </c>
+      <c r="C3" s="69" t="s">
+        <v>113</v>
+      </c>
+      <c r="D3" s="69" t="s">
+        <v>124</v>
+      </c>
+      <c r="E3" s="69" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="58" t="s">
+        <v>89</v>
+      </c>
+      <c r="B4" s="59"/>
+      <c r="C4" s="59"/>
+      <c r="D4" s="59"/>
+    </row>
+    <row r="5" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="70" t="s">
+        <v>111</v>
+      </c>
+      <c r="B5" s="69" t="s">
+        <v>115</v>
+      </c>
+      <c r="C5" s="69"/>
+      <c r="D5" s="69"/>
+      <c r="E5" s="69"/>
+    </row>
+    <row r="6" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="61" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" s="62"/>
+      <c r="C6" s="62"/>
+      <c r="D6" s="62"/>
+    </row>
+    <row r="7" spans="1:7" ht="159" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="C7" s="69" t="s">
+        <v>122</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="G7" s="78" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="58" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="59"/>
+      <c r="C8" s="59"/>
+      <c r="D8" s="59"/>
+      <c r="G8" s="79"/>
+    </row>
+    <row r="9" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A9" s="34" t="s">
+        <v>109</v>
+      </c>
+      <c r="B9" s="68" t="s">
+        <v>117</v>
+      </c>
+      <c r="C9" s="68" t="s">
+        <v>121</v>
+      </c>
+      <c r="D9" s="34" t="s">
+        <v>125</v>
+      </c>
+      <c r="E9" s="34" t="s">
+        <v>125</v>
+      </c>
+      <c r="G9" s="79" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="61" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10" s="62"/>
+      <c r="C10" s="62"/>
+      <c r="D10" s="62"/>
+      <c r="G10" s="80"/>
+    </row>
+    <row r="11" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A11" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="B11" s="73" t="s">
+        <v>118</v>
+      </c>
+      <c r="C11" s="69" t="s">
+        <v>113</v>
+      </c>
+      <c r="D11" s="67"/>
+      <c r="E11" s="67"/>
+      <c r="G11" s="79"/>
+    </row>
+    <row r="12" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="55" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="56"/>
+      <c r="C12" s="56"/>
+      <c r="D12" s="56"/>
+      <c r="G12" s="78"/>
+    </row>
+    <row r="13" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A13" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="66"/>
+      <c r="C13" s="69" t="s">
+        <v>120</v>
+      </c>
+      <c r="D13" s="66"/>
+      <c r="E13" s="66"/>
+      <c r="G13" s="78" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="55" t="s">
+        <v>112</v>
+      </c>
+      <c r="B14" s="56"/>
+      <c r="C14" s="56"/>
+      <c r="D14" s="56"/>
+    </row>
+    <row r="15" spans="1:7" ht="248" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="71" t="s">
+        <v>110</v>
+      </c>
+      <c r="B15" s="74" t="s">
+        <v>119</v>
+      </c>
+      <c r="C15" s="69" t="s">
+        <v>120</v>
+      </c>
+      <c r="D15" s="75" t="s">
+        <v>126</v>
+      </c>
+      <c r="E15" s="76" t="s">
+        <v>127</v>
+      </c>
+      <c r="F15" s="77" t="s">
+        <v>106</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A6:D6"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" display="WFP Proteus composite index: " xr:uid="{3B8342E4-A803-C342-923C-31BDAA92A373}"/>
+    <hyperlink ref="B11" r:id="rId2" xr:uid="{95E245AA-F0BF-3C40-B212-C5EC3EDEDF2E}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AE329EB-F042-854D-9101-2A27A77A5368}">
   <sheetPr>
-    <tabColor theme="5" tint="0.59999389629810485"/>
+    <tabColor rgb="FFC00000"/>
   </sheetPr>
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4745,46 +5939,46 @@
   <sheetData>
     <row r="1" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="23" t="s">
         <v>71</v>
-      </c>
-      <c r="B1" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="C1" s="23" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="38" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B2" s="39" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A3" s="38" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B3" s="39" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="38" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B4" s="39" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>